<commit_message>
I hope this is the end
</commit_message>
<xml_diff>
--- a/cp1/chyrkov_fb-05_cp1/letters_with_space.xlsx
+++ b/cp1/chyrkov_fb-05_cp1/letters_with_space.xlsx
@@ -16,16 +16,79 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
-    <t>{'в':</t>
+    <t>'</t>
+  </si>
+  <si>
+    <t>0.16870144486914324,</t>
+  </si>
+  <si>
+    <t>'о':</t>
+  </si>
+  <si>
+    <t>0.09294082394813964,</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>'е':</t>
+  </si>
+  <si>
+    <t>0.07304555320874961,</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>0.14089051896624727</t>
+  </si>
+  <si>
+    <t>'а':</t>
+  </si>
+  <si>
+    <t>0.06750213770472634,</t>
+  </si>
+  <si>
+    <t>'н':</t>
+  </si>
+  <si>
+    <t>0.055647925512866424,</t>
+  </si>
+  <si>
+    <t>'и':</t>
+  </si>
+  <si>
+    <t>0.05296209136951962,</t>
+  </si>
+  <si>
+    <t>'т':</t>
+  </si>
+  <si>
+    <t>0.05234087803024213,</t>
+  </si>
+  <si>
+    <t>'с':</t>
+  </si>
+  <si>
+    <t>0.04425048783518114,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'в':</t>
   </si>
   <si>
     <t>0.038663221977797105,</t>
   </si>
   <si>
-    <t>'</t>
-  </si>
-  <si>
-    <t>0.16870144486914324,</t>
+    <t>'л':</t>
+  </si>
+  <si>
+    <t>0.03860658193803945,</t>
+  </si>
+  <si>
+    <t>'р':</t>
+  </si>
+  <si>
+    <t>0.032787274627454704,</t>
   </si>
   <si>
     <t>'к':</t>
@@ -34,16 +97,112 @@
     <t>0.027234723633147943,</t>
   </si>
   <si>
-    <t>'о':</t>
-  </si>
-  <si>
-    <t>0.09294082394813964,</t>
-  </si>
-  <si>
-    <t>'н':</t>
-  </si>
-  <si>
-    <t>0.055647925512866424,</t>
+    <t>'д':</t>
+  </si>
+  <si>
+    <t>0.025853437502283874,</t>
+  </si>
+  <si>
+    <t>'м':</t>
+  </si>
+  <si>
+    <t>0.025541003734588428,</t>
+  </si>
+  <si>
+    <t>'п':</t>
+  </si>
+  <si>
+    <t>0.02260485715747393,</t>
+  </si>
+  <si>
+    <t>'у':</t>
+  </si>
+  <si>
+    <t>0.02175708365916582,</t>
+  </si>
+  <si>
+    <t>'я':</t>
+  </si>
+  <si>
+    <t>0.019900752033560138,</t>
+  </si>
+  <si>
+    <t>'ь':</t>
+  </si>
+  <si>
+    <t>0.018797184807314238,</t>
+  </si>
+  <si>
+    <t>'г':</t>
+  </si>
+  <si>
+    <t>0.015758720739024623,</t>
+  </si>
+  <si>
+    <t>'ч':</t>
+  </si>
+  <si>
+    <t>0.015316563009303584,</t>
+  </si>
+  <si>
+    <t>'ы':</t>
+  </si>
+  <si>
+    <t>0.014461481118768682,</t>
+  </si>
+  <si>
+    <t>'з':</t>
+  </si>
+  <si>
+    <t>0.014371953313990455,</t>
+  </si>
+  <si>
+    <t>'б':</t>
+  </si>
+  <si>
+    <t>0.013889599427022049,</t>
+  </si>
+  <si>
+    <t>'ъ':</t>
+  </si>
+  <si>
+    <t>0.0001827098056698507}</t>
+  </si>
+  <si>
+    <t>'ж':</t>
+  </si>
+  <si>
+    <t>0.009605054484064051,</t>
+  </si>
+  <si>
+    <t>'й':</t>
+  </si>
+  <si>
+    <t>0.008611113141220064,</t>
+  </si>
+  <si>
+    <t>'ш':</t>
+  </si>
+  <si>
+    <t>0.00692652873294404,</t>
+  </si>
+  <si>
+    <t>'х':</t>
+  </si>
+  <si>
+    <t>0.005877774448399097,</t>
+  </si>
+  <si>
+    <t>'ю':</t>
+  </si>
+  <si>
+    <t>0.0049441273414261595,</t>
+  </si>
+  <si>
+    <t>'э':</t>
+  </si>
+  <si>
+    <t>0.0029507633615680887,</t>
   </si>
   <si>
     <t>'ц':</t>
@@ -52,181 +211,22 @@
     <t>0.002707759320027187,</t>
   </si>
   <si>
-    <t>'е':</t>
-  </si>
-  <si>
-    <t>0.07304555320874961,</t>
-  </si>
-  <si>
-    <t>H1</t>
-  </si>
-  <si>
-    <t>'я':</t>
-  </si>
-  <si>
-    <t>0.019900752033560138,</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>0.14089051896624727</t>
-  </si>
-  <si>
-    <t>'б':</t>
-  </si>
-  <si>
-    <t>0.013889599427022049,</t>
-  </si>
-  <si>
-    <t>'р':</t>
-  </si>
-  <si>
-    <t>0.032787274627454704,</t>
-  </si>
-  <si>
-    <t>'т':</t>
-  </si>
-  <si>
-    <t>0.05234087803024213,</t>
-  </si>
-  <si>
-    <t>'п':</t>
-  </si>
-  <si>
-    <t>0.02260485715747393,</t>
-  </si>
-  <si>
-    <t>'л':</t>
-  </si>
-  <si>
-    <t>0.03860658193803945,</t>
-  </si>
-  <si>
-    <t>'ь':</t>
-  </si>
-  <si>
-    <t>0.018797184807314238,</t>
-  </si>
-  <si>
-    <t>'ч':</t>
-  </si>
-  <si>
-    <t>0.015316563009303584,</t>
-  </si>
-  <si>
-    <t>'а':</t>
-  </si>
-  <si>
-    <t>0.06750213770472634,</t>
-  </si>
-  <si>
-    <t>'с':</t>
-  </si>
-  <si>
-    <t>0.04425048783518114,</t>
-  </si>
-  <si>
-    <t>'д':</t>
-  </si>
-  <si>
-    <t>0.025853437502283874,</t>
-  </si>
-  <si>
-    <t>'у':</t>
-  </si>
-  <si>
-    <t>0.02175708365916582,</t>
-  </si>
-  <si>
-    <t>'з':</t>
-  </si>
-  <si>
-    <t>0.014371953313990455,</t>
-  </si>
-  <si>
-    <t>'г':</t>
-  </si>
-  <si>
-    <t>0.015758720739024623,</t>
-  </si>
-  <si>
-    <t>'ш':</t>
-  </si>
-  <si>
-    <t>0.00692652873294404,</t>
-  </si>
-  <si>
-    <t>'й':</t>
-  </si>
-  <si>
-    <t>0.008611113141220064,</t>
-  </si>
-  <si>
-    <t>'ъ':</t>
-  </si>
-  <si>
-    <t>0.0001827098056698507}</t>
-  </si>
-  <si>
-    <t>'ж':</t>
-  </si>
-  <si>
-    <t>0.009605054484064051,</t>
-  </si>
-  <si>
-    <t>'и':</t>
-  </si>
-  <si>
-    <t>0.05296209136951962,</t>
-  </si>
-  <si>
-    <t>'х':</t>
-  </si>
-  <si>
-    <t>0.005877774448399097,</t>
-  </si>
-  <si>
-    <t>'ы':</t>
-  </si>
-  <si>
-    <t>0.014461481118768682,</t>
-  </si>
-  <si>
-    <t>'м':</t>
-  </si>
-  <si>
-    <t>0.025541003734588428,</t>
-  </si>
-  <si>
     <t>'щ':</t>
   </si>
   <si>
     <t>0.0024537926901460946,</t>
   </si>
   <si>
+    <t>'ф':</t>
+  </si>
+  <si>
+    <t>0.0018362335469819995,</t>
+  </si>
+  <si>
     <t>'ё':</t>
   </si>
   <si>
     <t>0.0009683619700502086,</t>
-  </si>
-  <si>
-    <t>'ю':</t>
-  </si>
-  <si>
-    <t>0.0049441273414261595,</t>
-  </si>
-  <si>
-    <t>'ф':</t>
-  </si>
-  <si>
-    <t>0.0018362335469819995,</t>
-  </si>
-  <si>
-    <t>'э':</t>
-  </si>
-  <si>
-    <t>0.0029507633615680887,</t>
   </si>
 </sst>
 </file>
@@ -234,10 +234,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -248,6 +248,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -256,22 +264,67 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,45 +338,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -340,6 +354,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -349,14 +371,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -364,29 +386,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -401,187 +401,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -592,6 +592,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -658,21 +673,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -697,7 +697,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -715,138 +715,135 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1170,8 +1167,8 @@
   <sheetPr/>
   <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1187,71 +1184,71 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>4.37068756132508</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1">
-        <v>4370687561325080</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1470,6 +1467,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:B34">
+    <sortCondition ref="B1" descending="1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>